<commit_message>
Change keTL value to 0 for atezoli in parameters/Atezoli_Params
</commit_message>
<xml_diff>
--- a/parameters/Atezoli_Params.xlsx
+++ b/parameters/Atezoli_Params.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/TMDD_EndogenousLigand/pgm_ModelGH/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepo\TMDD_EndogenousLigand\parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF8E0D26-AF33-4DF9-AA71-77F146E21209}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2480" yWindow="460" windowWidth="24840" windowHeight="16180" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -104,10 +105,16 @@
     <definedName name="VtumDS">Sheet1!#REF!</definedName>
     <definedName name="VtumS">Sheet1!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -404,16 +411,16 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="0.000000"/>
-    <numFmt numFmtId="177" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -422,7 +429,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -430,33 +437,33 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <strike/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -575,7 +582,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -593,7 +600,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -637,31 +644,31 @@
     </xf>
   </cellXfs>
   <cellStyles count="25">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="13" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="35">
     <dxf>
@@ -1175,21 +1182,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J32" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J32" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J32" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="Order" dataDxfId="9"/>
-    <tableColumn id="2" name="ParamType" dataDxfId="8"/>
-    <tableColumn id="3" name="Molecule" dataDxfId="7"/>
-    <tableColumn id="4" name="Description" dataDxfId="6"/>
-    <tableColumn id="5" name="Parameter" dataDxfId="5"/>
-    <tableColumn id="6" name="Value" dataDxfId="4"/>
-    <tableColumn id="7" name="Units" dataDxfId="3"/>
-    <tableColumn id="8" name="Source" dataDxfId="2"/>
-    <tableColumn id="10" name="Formula" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Order" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ParamType" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Molecule" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Description" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Parameter" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Value" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Units" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Source" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Formula" dataDxfId="1">
       <calculatedColumnFormula>_xlfn.IFNA(_xlfn.FORMULATEXT(F2),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Comment or Reference" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Comment or Reference" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1516,29 +1523,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="8.5" style="3" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13.375" style="3" customWidth="1"/>
     <col min="3" max="3" width="20" style="3" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" style="21" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.125" style="21" customWidth="1"/>
+    <col min="7" max="7" width="9.875" style="1" customWidth="1"/>
     <col min="8" max="8" width="20" style="2" customWidth="1"/>
     <col min="9" max="9" width="25.5" style="2" customWidth="1"/>
-    <col min="10" max="10" width="50.33203125" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="4"/>
+    <col min="10" max="10" width="50.375" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="10.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10">
       <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
@@ -1570,7 +1577,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1603,7 +1610,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -1636,7 +1643,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" s="25" customFormat="1">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1669,7 +1676,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" s="25" customFormat="1">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1702,7 +1709,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" s="25" customFormat="1">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1735,7 +1742,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" s="25" customFormat="1">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1768,7 +1775,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" s="25" customFormat="1">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1800,7 +1807,7 @@
       </c>
       <c r="J8" s="24"/>
     </row>
-    <row r="9" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" s="25" customFormat="1">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1830,7 +1837,7 @@
       </c>
       <c r="J9" s="24"/>
     </row>
-    <row r="10" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" s="25" customFormat="1">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1860,7 +1867,7 @@
       </c>
       <c r="J10" s="24"/>
     </row>
-    <row r="11" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" s="25" customFormat="1">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1893,7 +1900,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" s="25" customFormat="1">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1926,7 +1933,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:10" s="25" customFormat="1">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1958,7 +1965,7 @@
       </c>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" s="25" customFormat="1">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1989,7 +1996,7 @@
       </c>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" s="25" customFormat="1">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -2022,7 +2029,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" s="25" customFormat="1">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -2055,7 +2062,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:10" s="25" customFormat="1">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -2088,7 +2095,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:10" s="25" customFormat="1">
       <c r="A18" s="2">
         <v>18</v>
       </c>
@@ -2120,7 +2127,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:10" s="25" customFormat="1">
       <c r="A19" s="2">
         <v>19</v>
       </c>
@@ -2153,7 +2160,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:10" s="25" customFormat="1">
       <c r="A20" s="30">
         <v>20</v>
       </c>
@@ -2186,7 +2193,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:10" s="25" customFormat="1">
       <c r="A21" s="2">
         <v>21</v>
       </c>
@@ -2219,7 +2226,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:10" s="25" customFormat="1">
       <c r="A22" s="2">
         <v>22</v>
       </c>
@@ -2252,7 +2259,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:10" s="25" customFormat="1">
       <c r="A23" s="2">
         <v>24</v>
       </c>
@@ -2285,7 +2292,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:10" s="25" customFormat="1">
       <c r="A24" s="2">
         <v>25</v>
       </c>
@@ -2316,7 +2323,7 @@
       </c>
       <c r="J24" s="8"/>
     </row>
-    <row r="25" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:10" s="25" customFormat="1">
       <c r="A25" s="2">
         <v>26</v>
       </c>
@@ -2348,7 +2355,7 @@
       </c>
       <c r="J25" s="8"/>
     </row>
-    <row r="26" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:10" s="25" customFormat="1">
       <c r="A26" s="2">
         <v>27</v>
       </c>
@@ -2378,7 +2385,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:10" s="25" customFormat="1">
       <c r="A27" s="2">
         <v>28</v>
       </c>
@@ -2411,7 +2418,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:10" s="25" customFormat="1">
       <c r="A28" s="2">
         <v>29</v>
       </c>
@@ -2428,7 +2435,7 @@
         <v>67</v>
       </c>
       <c r="F28" s="21">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>4</v>
@@ -2441,7 +2448,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:10" s="25" customFormat="1">
       <c r="A29" s="2">
         <v>30</v>
       </c>
@@ -2471,7 +2478,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:10">
       <c r="A30" s="6">
         <v>31</v>
       </c>
@@ -2502,7 +2509,7 @@
       </c>
       <c r="J30" s="7"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:10">
       <c r="A31" s="6">
         <v>32</v>
       </c>
@@ -2535,7 +2542,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:10">
       <c r="A32" s="6">
         <v>33</v>
       </c>

</xml_diff>